<commit_message>
fix email and da name
</commit_message>
<xml_diff>
--- a/example/STR-EXAMPLE.xlsx
+++ b/example/STR-EXAMPLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2792DA4-1CAA-E841-A6FE-B44F6C4DC0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4F6FDF-255D-9546-A6DE-54D7007E4D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -34,9 +34,6 @@
     <t>Study_ID</t>
   </si>
   <si>
-    <t>DEMO</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
@@ -103,10 +100,10 @@
     <t>example-kb:DPL-generic-questionnaire</t>
   </si>
   <si>
-    <t>example@exmaple.com</t>
-  </si>
-  <si>
     <t>EXAMPLE</t>
+  </si>
+  <si>
+    <t>example@example.com</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1388,7 +1385,7 @@
     </row>
     <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>5</v>
@@ -1399,10 +1396,10 @@
     </row>
     <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1410,10 +1407,10 @@
     </row>
     <row r="5" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1421,10 +1418,10 @@
     </row>
     <row r="6" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1472,7 +1469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1487,40 +1486,40 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1551,28 +1550,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1679,7 +1678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1690,16 +1689,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E1" s="3"/>
     </row>

</xml_diff>